<commit_message>
Projetos de Lei sobre Meio Ambiente e Agricultura
</commit_message>
<xml_diff>
--- a/leis_meio_ambiente_agricultura_camara.xlsx
+++ b/leis_meio_ambiente_agricultura_camara.xlsx
@@ -532,7 +532,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2299178</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -577,7 +581,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2218288</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -622,7 +630,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2230152</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -671,7 +683,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2224581</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -720,7 +736,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2220655</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -765,7 +785,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2227753</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -810,7 +834,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2221658</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -855,7 +883,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2205239</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -900,7 +932,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2207825</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -945,7 +981,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2205374</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -994,7 +1034,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2210926</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1039,7 +1083,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2190623</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1084,7 +1132,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2219094</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1129,7 +1181,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2228130</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1174,7 +1230,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2295246</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1219,7 +1279,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2210900</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1264,7 +1328,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2191922</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1309,7 +1377,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2231979</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1354,7 +1426,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2208912</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1399,7 +1475,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2209304</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1448,7 +1528,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=946475</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1493,7 +1577,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2198592</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1538,7 +1626,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2222610</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1583,7 +1675,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2195731</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1628,7 +1724,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2190630</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1673,7 +1773,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2203744</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1718,7 +1822,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2201526</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1763,7 +1871,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2191050</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1808,7 +1920,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2230578</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1853,7 +1969,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2244008</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1902,7 +2022,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2215702</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1947,7 +2071,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2190497</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1988,7 +2116,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2190945</t>
         </is>
       </c>
-      <c r="K34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2029,7 +2161,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2192576</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2070,7 +2206,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2226165</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr"/>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2111,7 +2251,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2206680</t>
         </is>
       </c>
-      <c r="K37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2152,7 +2296,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2195715</t>
         </is>
       </c>
-      <c r="K38" t="inlineStr"/>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2193,7 +2341,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2226591</t>
         </is>
       </c>
-      <c r="K39" t="inlineStr"/>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2238,7 +2390,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2230022</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr"/>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2283,7 +2439,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2192575</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2328,7 +2488,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2191516</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2377,7 +2541,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2217784</t>
         </is>
       </c>
-      <c r="K43" t="inlineStr"/>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2422,7 +2590,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2198329</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr"/>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2467,7 +2639,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2211133</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr"/>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2512,7 +2688,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2190944</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2557,7 +2737,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2192427</t>
         </is>
       </c>
-      <c r="K47" t="inlineStr"/>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2602,7 +2786,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2192577</t>
         </is>
       </c>
-      <c r="K48" t="inlineStr"/>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2647,7 +2835,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2217918</t>
         </is>
       </c>
-      <c r="K49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -2692,7 +2884,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2222507</t>
         </is>
       </c>
-      <c r="K50" t="inlineStr"/>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2737,7 +2933,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2206396</t>
         </is>
       </c>
-      <c r="K51" t="inlineStr"/>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2782,7 +2982,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2192606</t>
         </is>
       </c>
-      <c r="K52" t="inlineStr"/>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2827,7 +3031,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2192438</t>
         </is>
       </c>
-      <c r="K53" t="inlineStr"/>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2872,7 +3080,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2213976</t>
         </is>
       </c>
-      <c r="K54" t="inlineStr"/>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2917,7 +3129,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2221268</t>
         </is>
       </c>
-      <c r="K55" t="inlineStr"/>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2962,7 +3178,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2229710</t>
         </is>
       </c>
-      <c r="K56" t="inlineStr"/>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -3003,7 +3223,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2197568</t>
         </is>
       </c>
-      <c r="K57" t="inlineStr"/>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -3036,7 +3260,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2190805</t>
         </is>
       </c>
-      <c r="K58" t="inlineStr"/>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -3077,7 +3305,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2204123</t>
         </is>
       </c>
-      <c r="K59" t="inlineStr"/>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -3118,7 +3350,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2191876</t>
         </is>
       </c>
-      <c r="K60" t="inlineStr"/>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -3163,7 +3399,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2217903</t>
         </is>
       </c>
-      <c r="K61" t="inlineStr"/>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -3208,7 +3448,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2214946</t>
         </is>
       </c>
-      <c r="K62" t="inlineStr"/>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -3253,7 +3497,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2210921</t>
         </is>
       </c>
-      <c r="K63" t="inlineStr"/>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -3298,7 +3546,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2222006</t>
         </is>
       </c>
-      <c r="K64" t="inlineStr"/>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -3343,7 +3595,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2212180</t>
         </is>
       </c>
-      <c r="K65" t="inlineStr"/>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -3388,7 +3644,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2220059</t>
         </is>
       </c>
-      <c r="K66" t="inlineStr"/>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -3433,7 +3693,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2200684</t>
         </is>
       </c>
-      <c r="K67" t="inlineStr"/>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -3478,7 +3742,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2201529</t>
         </is>
       </c>
-      <c r="K68" t="inlineStr"/>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -3527,7 +3795,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2248001</t>
         </is>
       </c>
-      <c r="K69" t="inlineStr"/>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -3572,7 +3844,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2260507</t>
         </is>
       </c>
-      <c r="K70" t="inlineStr"/>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -3617,7 +3893,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2254081</t>
         </is>
       </c>
-      <c r="K71" t="inlineStr"/>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -3662,7 +3942,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2263522</t>
         </is>
       </c>
-      <c r="K72" t="inlineStr"/>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -3707,7 +3991,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2260427</t>
         </is>
       </c>
-      <c r="K73" t="inlineStr"/>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -3752,7 +4040,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2244200</t>
         </is>
       </c>
-      <c r="K74" t="inlineStr"/>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -3797,7 +4089,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2261163</t>
         </is>
       </c>
-      <c r="K75" t="inlineStr"/>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -3842,7 +4138,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2264139</t>
         </is>
       </c>
-      <c r="K76" t="inlineStr"/>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -3887,7 +4187,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2248221</t>
         </is>
       </c>
-      <c r="K77" t="inlineStr"/>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -3932,7 +4236,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2260475</t>
         </is>
       </c>
-      <c r="K78" t="inlineStr"/>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -3977,7 +4285,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2252780</t>
         </is>
       </c>
-      <c r="K79" t="inlineStr"/>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -4022,7 +4334,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2255001</t>
         </is>
       </c>
-      <c r="K80" t="inlineStr"/>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -4067,7 +4383,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2263079</t>
         </is>
       </c>
-      <c r="K81" t="inlineStr"/>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -4112,7 +4432,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2263447</t>
         </is>
       </c>
-      <c r="K82" t="inlineStr"/>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -4157,7 +4481,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2237082</t>
         </is>
       </c>
-      <c r="K83" t="inlineStr"/>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -4202,7 +4530,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2255162</t>
         </is>
       </c>
-      <c r="K84" t="inlineStr"/>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -4247,7 +4579,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2237146</t>
         </is>
       </c>
-      <c r="K85" t="inlineStr"/>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -4292,7 +4628,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2252659</t>
         </is>
       </c>
-      <c r="K86" t="inlineStr"/>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -4337,7 +4677,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2237751</t>
         </is>
       </c>
-      <c r="K87" t="inlineStr"/>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -4382,7 +4726,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2250797</t>
         </is>
       </c>
-      <c r="K88" t="inlineStr"/>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -4431,7 +4779,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2258616</t>
         </is>
       </c>
-      <c r="K89" t="inlineStr"/>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -4472,7 +4824,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2263069</t>
         </is>
       </c>
-      <c r="K90" t="inlineStr"/>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -4513,7 +4869,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2260661</t>
         </is>
       </c>
-      <c r="K91" t="inlineStr"/>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -4554,7 +4914,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2260458</t>
         </is>
       </c>
-      <c r="K92" t="inlineStr"/>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -4595,7 +4959,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2264637</t>
         </is>
       </c>
-      <c r="K93" t="inlineStr"/>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -4640,7 +5008,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2259355</t>
         </is>
       </c>
-      <c r="K94" t="inlineStr"/>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -4685,7 +5057,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2242315</t>
         </is>
       </c>
-      <c r="K95" t="inlineStr"/>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -4730,7 +5106,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2262110</t>
         </is>
       </c>
-      <c r="K96" t="inlineStr"/>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -4771,7 +5151,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2236732</t>
         </is>
       </c>
-      <c r="K97" t="inlineStr"/>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -4816,7 +5200,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2252648</t>
         </is>
       </c>
-      <c r="K98" t="inlineStr"/>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -4853,7 +5241,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2265117</t>
         </is>
       </c>
-      <c r="K99" t="inlineStr"/>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -4902,7 +5294,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2267546</t>
         </is>
       </c>
-      <c r="K100" t="inlineStr"/>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -4951,7 +5347,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2236972</t>
         </is>
       </c>
-      <c r="K101" t="inlineStr"/>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -4996,7 +5396,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2261263</t>
         </is>
       </c>
-      <c r="K102" t="inlineStr"/>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -5041,7 +5445,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2265092</t>
         </is>
       </c>
-      <c r="K103" t="inlineStr"/>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -5086,7 +5494,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2254168</t>
         </is>
       </c>
-      <c r="K104" t="inlineStr"/>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -5123,7 +5535,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2273620</t>
         </is>
       </c>
-      <c r="K105" t="inlineStr"/>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -5168,7 +5584,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2282842</t>
         </is>
       </c>
-      <c r="K106" t="inlineStr"/>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -5213,7 +5633,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2288806</t>
         </is>
       </c>
-      <c r="K107" t="inlineStr"/>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -5258,7 +5682,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2269804</t>
         </is>
       </c>
-      <c r="K108" t="inlineStr"/>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -5303,7 +5731,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2271972</t>
         </is>
       </c>
-      <c r="K109" t="inlineStr"/>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -5348,7 +5780,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2311272</t>
         </is>
       </c>
-      <c r="K110" t="inlineStr"/>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -5393,7 +5829,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2305360</t>
         </is>
       </c>
-      <c r="K111" t="inlineStr"/>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -5438,7 +5878,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2285651</t>
         </is>
       </c>
-      <c r="K112" t="inlineStr"/>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -5483,7 +5927,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2276014</t>
         </is>
       </c>
-      <c r="K113" t="inlineStr"/>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -5528,7 +5976,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2270256</t>
         </is>
       </c>
-      <c r="K114" t="inlineStr"/>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -5573,7 +6025,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2294110</t>
         </is>
       </c>
-      <c r="K115" t="inlineStr"/>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -5618,7 +6074,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2297396</t>
         </is>
       </c>
-      <c r="K116" t="inlineStr"/>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -5663,7 +6123,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2299148</t>
         </is>
       </c>
-      <c r="K117" t="inlineStr"/>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -5708,7 +6172,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2307296</t>
         </is>
       </c>
-      <c r="K118" t="inlineStr"/>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -5753,7 +6221,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2296630</t>
         </is>
       </c>
-      <c r="K119" t="inlineStr"/>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -5798,7 +6270,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2302889</t>
         </is>
       </c>
-      <c r="K120" t="inlineStr"/>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -5843,7 +6319,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2278601</t>
         </is>
       </c>
-      <c r="K121" t="inlineStr"/>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -5888,7 +6368,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2302345</t>
         </is>
       </c>
-      <c r="K122" t="inlineStr"/>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -5933,7 +6417,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2286335</t>
         </is>
       </c>
-      <c r="K123" t="inlineStr"/>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -5978,7 +6466,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2313055</t>
         </is>
       </c>
-      <c r="K124" t="inlineStr"/>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -6023,7 +6515,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2288135</t>
         </is>
       </c>
-      <c r="K125" t="inlineStr"/>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -6068,7 +6564,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2277436</t>
         </is>
       </c>
-      <c r="K126" t="inlineStr"/>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -6113,7 +6613,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2285328</t>
         </is>
       </c>
-      <c r="K127" t="inlineStr"/>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -6158,7 +6662,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2306247</t>
         </is>
       </c>
-      <c r="K128" t="inlineStr"/>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -6203,7 +6711,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2305375</t>
         </is>
       </c>
-      <c r="K129" t="inlineStr"/>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -6248,7 +6760,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2277160</t>
         </is>
       </c>
-      <c r="K130" t="inlineStr"/>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -6293,7 +6809,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2289048</t>
         </is>
       </c>
-      <c r="K131" t="inlineStr"/>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -6338,7 +6858,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2333780</t>
         </is>
       </c>
-      <c r="K132" t="inlineStr"/>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -6383,7 +6907,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2286124</t>
         </is>
       </c>
-      <c r="K133" t="inlineStr"/>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -6428,7 +6956,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2303865</t>
         </is>
       </c>
-      <c r="K134" t="inlineStr"/>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -6473,7 +7005,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2306715</t>
         </is>
       </c>
-      <c r="K135" t="inlineStr"/>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -6518,7 +7054,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2312467</t>
         </is>
       </c>
-      <c r="K136" t="inlineStr"/>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -6563,7 +7103,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2313315</t>
         </is>
       </c>
-      <c r="K137" t="inlineStr"/>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -6608,7 +7152,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2312878</t>
         </is>
       </c>
-      <c r="K138" t="inlineStr"/>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -6653,7 +7201,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2312591</t>
         </is>
       </c>
-      <c r="K139" t="inlineStr"/>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -6698,7 +7250,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2306599</t>
         </is>
       </c>
-      <c r="K140" t="inlineStr"/>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -6743,7 +7299,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2270420</t>
         </is>
       </c>
-      <c r="K141" t="inlineStr"/>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -6788,7 +7348,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2294450</t>
         </is>
       </c>
-      <c r="K142" t="inlineStr"/>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -6833,7 +7397,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2269461</t>
         </is>
       </c>
-      <c r="K143" t="inlineStr"/>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -6878,7 +7446,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2280256</t>
         </is>
       </c>
-      <c r="K144" t="inlineStr"/>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -6923,7 +7495,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2287916</t>
         </is>
       </c>
-      <c r="K145" t="inlineStr"/>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -6972,7 +7548,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2284430</t>
         </is>
       </c>
-      <c r="K146" t="inlineStr"/>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -7017,7 +7597,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2306829</t>
         </is>
       </c>
-      <c r="K147" t="inlineStr"/>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -7062,7 +7646,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2305853</t>
         </is>
       </c>
-      <c r="K148" t="inlineStr"/>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -7107,7 +7695,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2273586</t>
         </is>
       </c>
-      <c r="K149" t="inlineStr"/>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -7152,7 +7744,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2277897</t>
         </is>
       </c>
-      <c r="K150" t="inlineStr"/>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -7197,7 +7793,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2299587</t>
         </is>
       </c>
-      <c r="K151" t="inlineStr"/>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -7242,7 +7842,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2275679</t>
         </is>
       </c>
-      <c r="K152" t="inlineStr"/>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -7287,7 +7891,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2278134</t>
         </is>
       </c>
-      <c r="K153" t="inlineStr"/>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -7332,7 +7940,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2301598</t>
         </is>
       </c>
-      <c r="K154" t="inlineStr"/>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -7377,7 +7989,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2317346</t>
         </is>
       </c>
-      <c r="K155" t="inlineStr"/>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -7422,7 +8038,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2336609</t>
         </is>
       </c>
-      <c r="K156" t="inlineStr"/>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -7467,7 +8087,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2326159</t>
         </is>
       </c>
-      <c r="K157" t="inlineStr"/>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -7512,7 +8136,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2341456</t>
         </is>
       </c>
-      <c r="K158" t="inlineStr"/>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -7557,7 +8185,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2324721</t>
         </is>
       </c>
-      <c r="K159" t="inlineStr"/>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -7602,7 +8234,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2340300</t>
         </is>
       </c>
-      <c r="K160" t="inlineStr"/>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -7647,7 +8283,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2326733</t>
         </is>
       </c>
-      <c r="K161" t="inlineStr"/>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -7692,7 +8332,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2335042</t>
         </is>
       </c>
-      <c r="K162" t="inlineStr"/>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -7737,7 +8381,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2342277</t>
         </is>
       </c>
-      <c r="K163" t="inlineStr"/>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -7782,7 +8430,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2343129</t>
         </is>
       </c>
-      <c r="K164" t="inlineStr"/>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -7827,7 +8479,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2333160</t>
         </is>
       </c>
-      <c r="K165" t="inlineStr"/>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -7872,7 +8528,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2334222</t>
         </is>
       </c>
-      <c r="K166" t="inlineStr"/>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -7917,7 +8577,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2326312</t>
         </is>
       </c>
-      <c r="K167" t="inlineStr"/>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -7962,7 +8626,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2323683</t>
         </is>
       </c>
-      <c r="K168" t="inlineStr"/>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -8007,7 +8675,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2334784</t>
         </is>
       </c>
-      <c r="K169" t="inlineStr"/>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -8052,7 +8724,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2334223</t>
         </is>
       </c>
-      <c r="K170" t="inlineStr"/>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -8097,7 +8773,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2313996</t>
         </is>
       </c>
-      <c r="K171" t="inlineStr"/>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -8142,7 +8822,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2319622</t>
         </is>
       </c>
-      <c r="K172" t="inlineStr"/>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -8187,7 +8871,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2318674</t>
         </is>
       </c>
-      <c r="K173" t="inlineStr"/>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -8232,7 +8920,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2330607</t>
         </is>
       </c>
-      <c r="K174" t="inlineStr"/>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -8277,7 +8969,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2330749</t>
         </is>
       </c>
-      <c r="K175" t="inlineStr"/>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -8322,7 +9018,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2314247</t>
         </is>
       </c>
-      <c r="K176" t="inlineStr"/>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -8367,7 +9067,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2325594</t>
         </is>
       </c>
-      <c r="K177" t="inlineStr"/>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -8412,7 +9116,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2340304</t>
         </is>
       </c>
-      <c r="K178" t="inlineStr"/>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -8457,7 +9165,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2336610</t>
         </is>
       </c>
-      <c r="K179" t="inlineStr"/>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -8502,7 +9214,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2341572</t>
         </is>
       </c>
-      <c r="K180" t="inlineStr"/>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -8547,7 +9263,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2339036</t>
         </is>
       </c>
-      <c r="K181" t="inlineStr"/>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -8592,7 +9312,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2314561</t>
         </is>
       </c>
-      <c r="K182" t="inlineStr"/>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -8637,7 +9361,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2338689</t>
         </is>
       </c>
-      <c r="K183" t="inlineStr"/>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -8682,7 +9410,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2344905</t>
         </is>
       </c>
-      <c r="K184" t="inlineStr"/>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -8727,7 +9459,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2330616</t>
         </is>
       </c>
-      <c r="K185" t="inlineStr"/>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -8772,7 +9508,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2317622</t>
         </is>
       </c>
-      <c r="K186" t="inlineStr"/>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -8817,7 +9557,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2326562</t>
         </is>
       </c>
-      <c r="K187" t="inlineStr"/>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -8862,7 +9606,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2323092</t>
         </is>
       </c>
-      <c r="K188" t="inlineStr"/>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -8907,7 +9655,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2317584</t>
         </is>
       </c>
-      <c r="K189" t="inlineStr"/>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -8952,7 +9704,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2315490</t>
         </is>
       </c>
-      <c r="K190" t="inlineStr"/>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -8997,7 +9753,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2314763</t>
         </is>
       </c>
-      <c r="K191" t="inlineStr"/>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -9042,7 +9802,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2191915</t>
         </is>
       </c>
-      <c r="K192" t="inlineStr"/>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -9087,7 +9851,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2194435</t>
         </is>
       </c>
-      <c r="K193" t="inlineStr"/>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -9132,7 +9900,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2258739</t>
         </is>
       </c>
-      <c r="K194" t="inlineStr"/>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -9177,7 +9949,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2306369</t>
         </is>
       </c>
-      <c r="K195" t="inlineStr"/>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -9218,7 +9994,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2308223</t>
         </is>
       </c>
-      <c r="K196" t="inlineStr"/>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -9263,7 +10043,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2270639</t>
         </is>
       </c>
-      <c r="K197" t="inlineStr"/>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -9308,7 +10092,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2307775</t>
         </is>
       </c>
-      <c r="K198" t="inlineStr"/>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -9353,7 +10141,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2307466</t>
         </is>
       </c>
-      <c r="K199" t="inlineStr"/>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -9398,7 +10190,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2339661</t>
         </is>
       </c>
-      <c r="K200" t="inlineStr"/>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -9443,7 +10239,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2343129</t>
         </is>
       </c>
-      <c r="K201" t="inlineStr"/>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -9488,7 +10288,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2342991</t>
         </is>
       </c>
-      <c r="K202" t="inlineStr"/>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -9533,7 +10337,11 @@
           <t>/proposicoesWeb/fichadetramitacao?idProposicao=2313859</t>
         </is>
       </c>
-      <c r="K203" t="inlineStr"/>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>Meio Ambiente</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">

</xml_diff>